<commit_message>
drafts make metadata, adds todos on clean data, trouble shoots building edi
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_microhabitat_metadata.xlsx
+++ b/data-raw/metadata/feather_microhabitat_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C44212-28A5-4F75-BA5F-FE9A63C7DA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA272BD-8017-477A-A723-01552754E549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="92">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -300,15 +300,17 @@
   <si>
     <t>mini-snorkel-survey</t>
   </si>
+  <si>
+    <t>Identification number of micro habitat data table</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -369,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -394,23 +396,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -632,9 +628,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -711,7 +707,9 @@
       <c r="A2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -727,12 +725,8 @@
       <c r="I2" s="2"/>
       <c r="J2" s="5"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="3">
-        <v>18</v>
-      </c>
-      <c r="M2" s="3">
-        <v>4894</v>
-      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -769,12 +763,8 @@
       <c r="I3" s="2"/>
       <c r="J3" s="5"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="17">
-        <v>11</v>
-      </c>
-      <c r="M3" s="17">
-        <v>146</v>
-      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -793,7 +783,9 @@
       <c r="A4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -809,8 +801,8 @@
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="9"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="3"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -877,7 +869,7 @@
       <c r="A6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -896,7 +888,7 @@
         <v>66</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
@@ -904,7 +896,7 @@
       <c r="L6" s="10">
         <v>0</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="13">
         <v>3.38</v>
       </c>
       <c r="N6" s="1"/>
@@ -929,7 +921,7 @@
         <v>77</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>90</v>
@@ -977,7 +969,7 @@
         <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>90</v>
@@ -997,10 +989,10 @@
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="17">
+      <c r="L8" s="3">
         <v>0</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="3">
         <v>100</v>
       </c>
       <c r="N8" s="1"/>
@@ -1025,7 +1017,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>90</v>
@@ -1045,10 +1037,10 @@
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="17">
+      <c r="L9" s="3">
         <v>0</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="3">
         <v>100</v>
       </c>
       <c r="N9" s="1"/>
@@ -1073,7 +1065,7 @@
         <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>90</v>
@@ -1093,10 +1085,10 @@
       <c r="I10" s="2"/>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="17">
+      <c r="L10" s="3">
         <v>0</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="3">
         <v>100</v>
       </c>
       <c r="N10" s="1"/>
@@ -1121,7 +1113,7 @@
         <v>70</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>90</v>
@@ -1141,10 +1133,10 @@
       <c r="I11" s="2"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="17">
+      <c r="L11" s="3">
         <v>0</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="3">
         <v>100</v>
       </c>
       <c r="N11" s="1"/>
@@ -1169,7 +1161,7 @@
         <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>90</v>
@@ -1189,10 +1181,10 @@
       <c r="I12" s="2"/>
       <c r="J12" s="5"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="17">
+      <c r="L12" s="3">
         <v>0</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="3">
         <v>100</v>
       </c>
       <c r="N12" s="1"/>
@@ -1217,7 +1209,7 @@
         <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>90</v>
@@ -1237,10 +1229,10 @@
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="17">
+      <c r="L13" s="3">
         <v>0</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="3">
         <v>100</v>
       </c>
       <c r="N13" s="1"/>
@@ -1265,7 +1257,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>90</v>
@@ -1285,10 +1277,10 @@
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="17">
+      <c r="L14" s="3">
         <v>0</v>
       </c>
-      <c r="M14" s="17">
+      <c r="M14" s="3">
         <v>100</v>
       </c>
       <c r="N14" s="1"/>
@@ -1313,7 +1305,7 @@
         <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>90</v>
@@ -1333,10 +1325,10 @@
       <c r="I15" s="2"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="17">
+      <c r="L15" s="3">
         <v>0</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15" s="3">
         <v>40</v>
       </c>
       <c r="N15" s="1"/>
@@ -1361,7 +1353,7 @@
         <v>78</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>90</v>
@@ -1381,10 +1373,10 @@
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="13">
+      <c r="L16" s="10">
         <v>0</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="10">
         <v>100</v>
       </c>
       <c r="N16" s="1"/>
@@ -1409,7 +1401,7 @@
         <v>79</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>90</v>
@@ -1457,7 +1449,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>90</v>
@@ -1505,7 +1497,7 @@
         <v>82</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>90</v>
@@ -1553,7 +1545,7 @@
         <v>81</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>90</v>
@@ -1783,7 +1775,7 @@
         <v>88</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>90</v>
@@ -1929,10 +1921,10 @@
         <v>33</v>
       </c>
       <c r="K28" s="2"/>
-      <c r="L28" s="15">
+      <c r="L28" s="14">
         <v>36963</v>
       </c>
-      <c r="M28" s="15">
+      <c r="M28" s="14">
         <v>37125</v>
       </c>
       <c r="N28" s="1"/>
@@ -29469,7 +29461,7 @@
       <c r="B3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="8"/>

</xml_diff>

<commit_message>
updates field descriptions and deletes TODOs
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_microhabitat_metadata.xlsx
+++ b/data-raw/metadata/feather_microhabitat_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA272BD-8017-477A-A723-01552754E549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A45655-9C5C-49E1-83CA-49A5A47B4C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37560" yWindow="0" windowWidth="22290" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="93">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -256,9 +256,6 @@
     <t>Geomorphic features of stream. Levels = c("Glide", "Glide Edgewater", "Pool", "Riffle Riffle Edgewaterl")</t>
   </si>
   <si>
-    <t xml:space="preserve">unsure </t>
-  </si>
-  <si>
     <t>Percetage of  fine substrate at survey location</t>
   </si>
   <si>
@@ -302,6 +299,12 @@
   </si>
   <si>
     <t>Identification number of micro habitat data table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code to identify specific one-meter transect surveyed </t>
+  </si>
+  <si>
+    <t>Unique identifier number for fish observations</t>
   </si>
 </sst>
 </file>
@@ -628,9 +631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -708,13 +711,13 @@
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>34</v>
@@ -752,7 +755,7 @@
         <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>34</v>
@@ -784,13 +787,13 @@
         <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>34</v>
@@ -828,7 +831,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -837,7 +840,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>17</v>
@@ -876,7 +879,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>16</v>
@@ -918,13 +921,13 @@
         <v>42</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -972,7 +975,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
@@ -1020,7 +1023,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
@@ -1068,7 +1071,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>16</v>
@@ -1116,7 +1119,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -1164,7 +1167,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
@@ -1203,16 +1206,16 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -1260,7 +1263,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
@@ -1308,7 +1311,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1350,13 +1353,13 @@
         <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>16</v>
@@ -1398,13 +1401,13 @@
         <v>51</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>16</v>
@@ -1446,13 +1449,13 @@
         <v>52</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>16</v>
@@ -1494,13 +1497,13 @@
         <v>53</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1542,13 +1545,13 @@
         <v>54</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>16</v>
@@ -1596,7 +1599,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>16</v>
@@ -1638,13 +1641,13 @@
         <v>56</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>34</v>
@@ -1682,7 +1685,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>16</v>
@@ -1730,7 +1733,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>16</v>
@@ -1769,16 +1772,16 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>16</v>
@@ -1787,7 +1790,7 @@
         <v>15</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>17</v>
@@ -1826,7 +1829,7 @@
         <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>16</v>
@@ -1870,7 +1873,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
@@ -1899,16 +1902,16 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>27</v>
@@ -1952,7 +1955,7 @@
         <v>13</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
fixes metadata error, adds more custom units
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_microhabitat_metadata.xlsx
+++ b/data-raw/metadata/feather_microhabitat_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66336755-CC9E-4F89-8028-C82ED2D8C58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7D590C-305A-40BA-99F6-B63FCCAFDB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,9 +196,6 @@
     <t>focal_velocity</t>
   </si>
   <si>
-    <t>species </t>
-  </si>
-  <si>
     <t>channel_geomorphic_unit</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>Where the focal velocity is taken from, where the fish was observed </t>
   </si>
   <si>
-    <t>feet</t>
-  </si>
-  <si>
     <t>mini-snorkel-survey</t>
   </si>
   <si>
@@ -295,7 +289,13 @@
     <t>Geomorphic features of stream. Features include = c("Glide", "Glide Edgewater", "Pool", "Riffle Riffle Edgewater")</t>
   </si>
   <si>
-    <t>Fish species. Species = c("Chinook salmon", "Speckled dace", "Steelhead trout  (wild)", " Steelhead trout,  (clipped)", "Tule perch")</t>
+    <t>Fish species. Species = c("Chinook salmon", "Speckled dace", "Steelhead trout (wild)", " Steelhead trout, (clipped)", "Tule perch")</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>meter</t>
   </si>
 </sst>
 </file>
@@ -622,9 +622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -702,13 +702,13 @@
         <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>33</v>
@@ -740,13 +740,13 @@
         <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>33</v>
@@ -778,13 +778,13 @@
         <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>33</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>25</v>
@@ -822,7 +822,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -831,7 +831,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>17</v>
@@ -864,13 +864,13 @@
         <v>38</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>16</v>
@@ -879,7 +879,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>31</v>
@@ -912,13 +912,13 @@
         <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -927,7 +927,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>17</v>
@@ -960,13 +960,13 @@
         <v>40</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
@@ -975,7 +975,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>17</v>
@@ -1008,13 +1008,13 @@
         <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
@@ -1023,7 +1023,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>17</v>
@@ -1056,13 +1056,13 @@
         <v>42</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>16</v>
@@ -1071,7 +1071,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>17</v>
@@ -1104,13 +1104,13 @@
         <v>43</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -1119,7 +1119,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>17</v>
@@ -1152,13 +1152,13 @@
         <v>44</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
@@ -1167,7 +1167,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>17</v>
@@ -1197,16 +1197,16 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -1215,7 +1215,7 @@
         <v>15</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>17</v>
@@ -1248,13 +1248,13 @@
         <v>45</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
@@ -1263,7 +1263,7 @@
         <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>17</v>
@@ -1296,13 +1296,13 @@
         <v>46</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1311,7 +1311,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1344,13 +1344,13 @@
         <v>47</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>16</v>
@@ -1359,7 +1359,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>17</v>
@@ -1392,13 +1392,13 @@
         <v>48</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>16</v>
@@ -1407,7 +1407,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>17</v>
@@ -1440,13 +1440,13 @@
         <v>49</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>16</v>
@@ -1455,7 +1455,7 @@
         <v>15</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>17</v>
@@ -1488,13 +1488,13 @@
         <v>50</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1503,7 +1503,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>17</v>
@@ -1536,13 +1536,13 @@
         <v>51</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>16</v>
@@ -1551,7 +1551,7 @@
         <v>15</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>17</v>
@@ -1590,7 +1590,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>16</v>
@@ -1632,13 +1632,13 @@
         <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>33</v>
@@ -1676,7 +1676,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>16</v>
@@ -1724,7 +1724,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>16</v>
@@ -1763,16 +1763,16 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>16</v>
@@ -1781,7 +1781,7 @@
         <v>15</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>17</v>
@@ -1814,13 +1814,13 @@
         <v>55</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>16</v>
@@ -1829,7 +1829,7 @@
         <v>15</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>17</v>
@@ -1855,16 +1855,16 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
@@ -1893,16 +1893,16 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>26</v>
@@ -1937,16 +1937,16 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
checks for errors and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_microhabitat_metadata.xlsx
+++ b/data-raw/metadata/feather_microhabitat_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7D590C-305A-40BA-99F6-B63FCCAFDB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC62CB57-EFC1-4972-9B74-61A078D1901B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="91">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -297,6 +297,9 @@
   <si>
     <t>meter</t>
   </si>
+  <si>
+    <t>Feather River ini-Snorkel Survey</t>
+  </si>
 </sst>
 </file>
 
@@ -365,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -398,9 +401,6 @@
     </xf>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -622,9 +622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -863,7 +863,7 @@
       <c r="A6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>60</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1837,8 +1837,12 @@
       <c r="I26" s="2"/>
       <c r="J26" s="3"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
+      <c r="L26" s="13">
+        <v>0</v>
+      </c>
+      <c r="M26" s="3">
+        <v>3.44</v>
+      </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -29369,7 +29373,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -29415,9 +29419,15 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -29443,9 +29453,15 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="15"/>
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -29471,9 +29487,15 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -29499,9 +29521,15 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>

</xml_diff>

<commit_message>
modifies id fields code definitions in metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_microhabitat_metadata.xlsx
+++ b/data-raw/metadata/feather_microhabitat_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC62CB57-EFC1-4972-9B74-61A078D1901B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56BF459-FD91-4C0A-9121-B624DE08FEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2410" yWindow="2160" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="94">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -115,9 +115,6 @@
     <t>millimeter</t>
   </si>
   <si>
-    <t>ordinal</t>
-  </si>
-  <si>
     <t>count of fish</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
   </si>
   <si>
     <t>YYYY-MM-DD</t>
-  </si>
-  <si>
-    <t>enumerated</t>
   </si>
   <si>
     <t>NTU</t>
@@ -298,7 +292,22 @@
     <t>meter</t>
   </si>
   <si>
-    <t>Feather River ini-Snorkel Survey</t>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>enumerated</t>
+  </si>
+  <si>
+    <t>18 - 4894</t>
+  </si>
+  <si>
+    <t>11-146</t>
+  </si>
+  <si>
+    <t>0.100 - 24.400</t>
+  </si>
+  <si>
+    <t>11 - 424</t>
   </si>
 </sst>
 </file>
@@ -622,9 +631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -699,19 +708,19 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
@@ -737,19 +746,19 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -775,19 +784,19 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -813,7 +822,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>25</v>
@@ -822,7 +831,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -831,7 +840,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>17</v>
@@ -861,16 +870,16 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>16</v>
@@ -879,10 +888,10 @@
         <v>15</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
@@ -909,16 +918,16 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -927,7 +936,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>17</v>
@@ -957,16 +966,16 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
@@ -975,7 +984,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>17</v>
@@ -1005,16 +1014,16 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
@@ -1023,7 +1032,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>17</v>
@@ -1053,16 +1062,16 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>16</v>
@@ -1071,7 +1080,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>17</v>
@@ -1101,16 +1110,16 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -1119,7 +1128,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>17</v>
@@ -1149,16 +1158,16 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
@@ -1167,7 +1176,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>17</v>
@@ -1197,16 +1206,16 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -1215,7 +1224,7 @@
         <v>15</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>17</v>
@@ -1245,16 +1254,16 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
@@ -1263,7 +1272,7 @@
         <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>17</v>
@@ -1293,16 +1302,16 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1311,7 +1320,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1341,16 +1350,16 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>16</v>
@@ -1359,7 +1368,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>17</v>
@@ -1389,16 +1398,16 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>16</v>
@@ -1407,7 +1416,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>17</v>
@@ -1437,16 +1446,16 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>16</v>
@@ -1455,7 +1464,7 @@
         <v>15</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>17</v>
@@ -1485,16 +1494,16 @@
     </row>
     <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1503,7 +1512,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>17</v>
@@ -1533,16 +1542,16 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>16</v>
@@ -1551,7 +1560,7 @@
         <v>15</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>17</v>
@@ -1581,7 +1590,7 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>22</v>
@@ -1590,7 +1599,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>16</v>
@@ -1599,7 +1608,7 @@
         <v>15</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>17</v>
@@ -1629,19 +1638,19 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1676,7 +1685,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>16</v>
@@ -1685,10 +1694,10 @@
         <v>15</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="5"/>
@@ -1715,7 +1724,7 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>27</v>
@@ -1724,7 +1733,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>16</v>
@@ -1763,16 +1772,16 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>16</v>
@@ -1781,7 +1790,7 @@
         <v>15</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>17</v>
@@ -1811,16 +1820,16 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>16</v>
@@ -1829,7 +1838,7 @@
         <v>15</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>17</v>
@@ -1859,16 +1868,16 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
@@ -1897,16 +1906,16 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>26</v>
@@ -1916,7 +1925,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="2"/>
       <c r="J28" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="14">
@@ -1941,16 +1950,16 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>
@@ -29373,7 +29382,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -29419,14 +29428,14 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="8" t="s">
         <v>90</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="C2" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -29453,14 +29462,14 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8">
-        <v>2</v>
+      <c r="A3" s="8" t="s">
+        <v>91</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>90</v>
+      <c r="B3" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -29487,14 +29496,14 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
-        <v>3</v>
+      <c r="A4" s="8" t="s">
+        <v>92</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>90</v>
+      <c r="B4" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -29521,16 +29530,15 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
-        <v>4</v>
+      <c r="A5" s="8" t="s">
+        <v>93</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>90</v>
+      <c r="B5" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
-      <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -57416,6 +57424,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes id fields to nominal-text in metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_microhabitat_metadata.xlsx
+++ b/data-raw/metadata/feather_microhabitat_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973464BA-41B8-4626-9D1E-BAD3577E099B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B748A0A-4B76-4E9B-A1E0-1E32CDAB66CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="88">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -230,24 +230,6 @@
   </si>
   <si>
     <t>meter</t>
-  </si>
-  <si>
-    <t>ordinal</t>
-  </si>
-  <si>
-    <t>enumerated</t>
-  </si>
-  <si>
-    <t>18 - 4894</t>
-  </si>
-  <si>
-    <t>11-146</t>
-  </si>
-  <si>
-    <t>0.100 - 24.400</t>
-  </si>
-  <si>
-    <t>11 - 424</t>
   </si>
   <si>
     <t>Depth of water in meters</t>
@@ -631,9 +613,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -714,13 +696,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
@@ -752,13 +734,13 @@
         <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -790,13 +772,13 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -825,7 +807,7 @@
         <v>52</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -921,7 +903,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -969,7 +951,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
@@ -1017,7 +999,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -1065,7 +1047,7 @@
         <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -1113,7 +1095,7 @@
         <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
@@ -1161,7 +1143,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
@@ -1209,7 +1191,7 @@
         <v>58</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
@@ -1257,7 +1239,7 @@
         <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -1305,7 +1287,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
@@ -1353,7 +1335,7 @@
         <v>42</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
@@ -1401,7 +1383,7 @@
         <v>43</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
@@ -1449,7 +1431,7 @@
         <v>44</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -1497,7 +1479,7 @@
         <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -1545,7 +1527,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
@@ -1593,7 +1575,7 @@
         <v>47</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>15</v>
@@ -1644,13 +1626,13 @@
         <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1727,7 +1709,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>15</v>
@@ -1775,7 +1757,7 @@
         <v>59</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>15</v>
@@ -1871,7 +1853,7 @@
         <v>66</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
@@ -1953,7 +1935,7 @@
         <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>13</v>
@@ -29381,8 +29363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -29428,15 +29410,9 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="A2" s="8"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -29462,15 +29438,9 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>31</v>
-      </c>
+      <c r="A3" s="8"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -29496,15 +29466,9 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>32</v>
-      </c>
+      <c r="A4" s="8"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -29530,15 +29494,9 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>48</v>
-      </c>
+      <c r="A5" s="8"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="11"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>

</xml_diff>

<commit_message>
updates to clean up location names and CGU
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_microhabitat_metadata.xlsx
+++ b/data-raw/metadata/feather_microhabitat_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/feather-mini-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D49DEC-9E18-5C47-BD9A-5B0336000D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE91BC7C-8CA5-C74F-858B-134694D64645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28840" yWindow="500" windowWidth="31660" windowHeight="27300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,9 +193,6 @@
     <t>Velocity specific to where fish was observed</t>
   </si>
   <si>
-    <t>Measured stream velocity (ft/s)</t>
-  </si>
-  <si>
     <t>feetPerSecond</t>
   </si>
   <si>
@@ -220,16 +217,10 @@
     <t xml:space="preserve">Code to identify specific one-meter transect surveyed </t>
   </si>
   <si>
-    <t>Unique identifier number for fish observations</t>
-  </si>
-  <si>
     <t>species</t>
   </si>
   <si>
     <t>meter</t>
-  </si>
-  <si>
-    <t>Depth of water in meters</t>
   </si>
   <si>
     <t>Percentage of  fine substrate at survey location</t>
@@ -290,6 +281,15 @@
   </si>
   <si>
     <t>Fork length of fish (mm)</t>
+  </si>
+  <si>
+    <t>Unique identifier number for fish observations. This field only exists for fish observations.</t>
+  </si>
+  <si>
+    <t>Depth of water in meters at the centerpoint of the section</t>
+  </si>
+  <si>
+    <t>Measured stream velocity (ft/s) at the centerpoint of the section</t>
   </si>
 </sst>
 </file>
@@ -615,7 +615,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -693,13 +693,13 @@
         <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -737,7 +737,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
@@ -769,13 +769,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -807,13 +807,13 @@
         <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -842,16 +842,16 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
@@ -895,7 +895,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -934,16 +934,16 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>14</v>
@@ -975,13 +975,13 @@
         <v>49</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
@@ -1020,16 +1020,16 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>16</v>
@@ -1038,7 +1038,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>17</v>
@@ -1071,13 +1071,13 @@
         <v>52</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -1086,7 +1086,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>17</v>
@@ -1125,7 +1125,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>16</v>
@@ -1134,7 +1134,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>17</v>
@@ -1167,13 +1167,13 @@
         <v>33</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>16</v>
@@ -1182,7 +1182,7 @@
         <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>27</v>
@@ -1215,13 +1215,13 @@
         <v>47</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
@@ -1263,13 +1263,13 @@
         <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1278,7 +1278,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1311,13 +1311,13 @@
         <v>35</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>16</v>
@@ -1326,7 +1326,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>17</v>
@@ -1359,13 +1359,13 @@
         <v>36</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>16</v>
@@ -1374,7 +1374,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>17</v>
@@ -1407,13 +1407,13 @@
         <v>37</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>16</v>
@@ -1422,7 +1422,7 @@
         <v>15</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>17</v>
@@ -1455,13 +1455,13 @@
         <v>38</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1470,7 +1470,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>17</v>
@@ -1503,13 +1503,13 @@
         <v>39</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>16</v>
@@ -1518,7 +1518,7 @@
         <v>15</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>17</v>
@@ -1548,16 +1548,16 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>16</v>
@@ -1566,7 +1566,7 @@
         <v>15</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>17</v>
@@ -1599,13 +1599,13 @@
         <v>40</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>16</v>
@@ -1614,7 +1614,7 @@
         <v>15</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>17</v>
@@ -1647,13 +1647,13 @@
         <v>41</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>16</v>
@@ -1662,7 +1662,7 @@
         <v>15</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>17</v>
@@ -1695,13 +1695,13 @@
         <v>42</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>16</v>
@@ -1710,7 +1710,7 @@
         <v>15</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>17</v>
@@ -1743,13 +1743,13 @@
         <v>43</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>16</v>
@@ -1758,7 +1758,7 @@
         <v>15</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>17</v>
@@ -1791,13 +1791,13 @@
         <v>44</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>16</v>
@@ -1806,7 +1806,7 @@
         <v>15</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>17</v>
@@ -1839,13 +1839,13 @@
         <v>45</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>16</v>
@@ -1854,7 +1854,7 @@
         <v>15</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>17</v>
@@ -1887,13 +1887,13 @@
         <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>16</v>
@@ -1902,7 +1902,7 @@
         <v>15</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>17</v>
@@ -1935,13 +1935,13 @@
         <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>

</xml_diff>